<commit_message>
Added test cases for OnlineCustomer
</commit_message>
<xml_diff>
--- a/TestDocuments/BMV_SOA_Test_Cases_V0.4.xlsx
+++ b/TestDocuments/BMV_SOA_Test_Cases_V0.4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="535" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="535" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Document History" sheetId="6" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2987" uniqueCount="985">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3025" uniqueCount="1001">
   <si>
     <t>S. No</t>
   </si>
@@ -7493,12 +7493,85 @@
     <t>FIRSTNAME = QWERTY                   postCode = SL11UW
 AND matchingCondition = EXACT</t>
   </si>
+  <si>
+    <t>OnlineCustomer.getPersonalProfile</t>
+  </si>
+  <si>
+    <t>OnlineCustomer.getPortalSubscriberlProfile</t>
+  </si>
+  <si>
+    <t>Customer sends a request to getPortalSubscriberlProfile details with input as below
+1. Customer ID
+2. AuthToken
+3.disambiguationID</t>
+  </si>
+  <si>
+    <t>Customer sends a request to getPortalSubscriberlProfile details with input as below
+1. Customer ID
+2. AuthToken</t>
+  </si>
+  <si>
+    <t>Customer sends a request to getPortalSubscriberlProfile details with input as below
+1. Customer ID</t>
+  </si>
+  <si>
+    <t>Customer sends a request to getPortalSubscriberlProfile details with input as below
+1.  AuthToken</t>
+  </si>
+  <si>
+    <t>Customer sends a request to getPortalSubscriberlProfile details with input as below
+1. Customer ID  - INVALID
+2. AuthToken  - VALID</t>
+  </si>
+  <si>
+    <t>Customer sends a request to getPortalSubscriberlProfile details with input as below
+1. Customer ID  - VALID
+2. AuthToken  - INVALID</t>
+  </si>
+  <si>
+    <t>Customer sends a request to getPortalSubscriberlProfile details with input as below
+1. Customer ID  - VALID
+2. AuthToken  - VALID
+3. disambiguationID  - INVALID</t>
+  </si>
+  <si>
+    <t>Returns profile and subscriber profile for single portal ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System should return with validation error and code should be 
+</t>
+  </si>
+  <si>
+    <t>Customer sends a request to getPortalSubscriberlProfile details with input as below
+1.disambiguationID</t>
+  </si>
+  <si>
+    <t>System should retun with error
+ErrorCode:
+Message:  Authentication failed due to incorrect customerid or authtoken</t>
+  </si>
+  <si>
+    <t>System should retun with error
+ErrorCode:
+Message:  Failed to retrieve user details</t>
+  </si>
+  <si>
+    <t>System should retun with error
+ErrorCode:
+Message:  Invalid disambiguationID</t>
+  </si>
+  <si>
+    <t>Customer sends a request to getPortalSubscriberlProfile details with input as below
+1. Customer ID  - INVALID
+2. AuthToken  - INVALID
+3. disambiguationID  - VALID</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7625,6 +7698,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -7676,7 +7755,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -7763,11 +7842,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -7959,8 +8084,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -7986,17 +8117,29 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8404,12 +8547,12 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
@@ -8580,28 +8723,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="77"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
     </row>
     <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="52" t="s">
@@ -8757,28 +8900,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="77"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
     </row>
     <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="52" t="s">
@@ -8972,28 +9115,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="77"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
     </row>
     <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="52" t="s">
@@ -9186,28 +9329,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="77"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
     </row>
     <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="52" t="s">
@@ -9400,28 +9543,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>826</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="77"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
     </row>
     <row r="3" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="52" t="s">
@@ -9596,28 +9739,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="77"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
     </row>
     <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
@@ -10708,28 +10851,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="77"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
     </row>
     <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
@@ -11228,28 +11371,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="77"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
     </row>
     <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
@@ -11676,28 +11819,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="77"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
     </row>
     <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
@@ -11729,17 +11872,17 @@
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="82" t="s">
         <v>119</v>
       </c>
-      <c r="B4" s="81"/>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="82"/>
     </row>
     <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
@@ -12452,17 +12595,17 @@
       </c>
     </row>
     <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="82" t="s">
+      <c r="A43" s="83" t="s">
         <v>147</v>
       </c>
-      <c r="B43" s="82"/>
-      <c r="C43" s="82"/>
-      <c r="D43" s="82"/>
-      <c r="E43" s="82"/>
-      <c r="F43" s="82"/>
-      <c r="G43" s="82"/>
-      <c r="H43" s="82"/>
-      <c r="I43" s="82"/>
+      <c r="B43" s="83"/>
+      <c r="C43" s="83"/>
+      <c r="D43" s="83"/>
+      <c r="E43" s="83"/>
+      <c r="F43" s="83"/>
+      <c r="G43" s="83"/>
+      <c r="H43" s="83"/>
+      <c r="I43" s="83"/>
     </row>
     <row r="44" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="32">
@@ -13046,28 +13189,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>398</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="77"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
     </row>
     <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
@@ -15089,7 +15232,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A34" sqref="A34:A38"/>
     </sheetView>
@@ -15108,28 +15251,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="73" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="80"/>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
+      <c r="A2" s="73"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="50" t="s">
@@ -15200,7 +15343,7 @@
         <v>183</v>
       </c>
       <c r="H5" s="23"/>
-      <c r="I5" s="83" t="s">
+      <c r="I5" s="71" t="s">
         <v>180</v>
       </c>
     </row>
@@ -16628,30 +16771,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="74" t="s">
         <v>275</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="72"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
     </row>
     <row r="3" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
@@ -17904,28 +18047,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="74" t="s">
         <v>319</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="72"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
     </row>
     <row r="3" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
@@ -18089,11 +18232,11 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I125"/>
+  <dimension ref="A1:I126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H64" sqref="H64"/>
+      <pane ySplit="3" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18110,28 +18253,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="78" t="s">
         <v>331</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="76"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
+      <c r="A2" s="78"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
     </row>
     <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
@@ -18162,20 +18305,20 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="73" t="s">
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="75" t="s">
         <v>825</v>
       </c>
-      <c r="B4" s="74"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="75"/>
-    </row>
-    <row r="5" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="77"/>
+    </row>
+    <row r="5" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -18198,7 +18341,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>2</v>
       </c>
@@ -18217,7 +18360,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>3</v>
       </c>
@@ -18236,7 +18379,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>4</v>
       </c>
@@ -18255,7 +18398,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>5</v>
       </c>
@@ -18274,7 +18417,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>6</v>
       </c>
@@ -18293,7 +18436,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>7</v>
       </c>
@@ -18312,7 +18455,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>8</v>
       </c>
@@ -18331,7 +18474,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>9</v>
       </c>
@@ -18350,20 +18493,20 @@
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="73" t="s">
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="75" t="s">
         <v>807</v>
       </c>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="74"/>
-      <c r="H14" s="74"/>
-      <c r="I14" s="75"/>
-    </row>
-    <row r="15" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="76"/>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
+      <c r="H14" s="76"/>
+      <c r="I14" s="77"/>
+    </row>
+    <row r="15" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>10</v>
       </c>
@@ -18382,7 +18525,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>11</v>
       </c>
@@ -18401,7 +18544,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>12</v>
       </c>
@@ -18420,7 +18563,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>13</v>
       </c>
@@ -18439,7 +18582,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>14</v>
       </c>
@@ -18458,7 +18601,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>15</v>
       </c>
@@ -18477,7 +18620,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>16</v>
       </c>
@@ -18496,7 +18639,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>17</v>
       </c>
@@ -18515,7 +18658,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>18</v>
       </c>
@@ -18534,20 +18677,20 @@
         <v>180</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="73" t="s">
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="75" t="s">
         <v>809</v>
       </c>
-      <c r="B24" s="74"/>
-      <c r="C24" s="74"/>
-      <c r="D24" s="74"/>
-      <c r="E24" s="74"/>
-      <c r="F24" s="74"/>
-      <c r="G24" s="74"/>
-      <c r="H24" s="74"/>
-      <c r="I24" s="75"/>
-    </row>
-    <row r="25" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="76"/>
+      <c r="C24" s="76"/>
+      <c r="D24" s="76"/>
+      <c r="E24" s="76"/>
+      <c r="F24" s="76"/>
+      <c r="G24" s="76"/>
+      <c r="H24" s="76"/>
+      <c r="I24" s="77"/>
+    </row>
+    <row r="25" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>19</v>
       </c>
@@ -18566,7 +18709,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>20</v>
       </c>
@@ -18585,7 +18728,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>21</v>
       </c>
@@ -18604,7 +18747,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>22</v>
       </c>
@@ -18623,7 +18766,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>23</v>
       </c>
@@ -18642,7 +18785,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>24</v>
       </c>
@@ -18661,7 +18804,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>25</v>
       </c>
@@ -18680,7 +18823,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>26</v>
       </c>
@@ -18699,7 +18842,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>27</v>
       </c>
@@ -18718,20 +18861,20 @@
         <v>180</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="73" t="s">
+    <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="75" t="s">
         <v>811</v>
       </c>
-      <c r="B34" s="74"/>
-      <c r="C34" s="74"/>
-      <c r="D34" s="74"/>
-      <c r="E34" s="74"/>
-      <c r="F34" s="74"/>
-      <c r="G34" s="74"/>
-      <c r="H34" s="74"/>
-      <c r="I34" s="75"/>
-    </row>
-    <row r="35" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="76"/>
+      <c r="C34" s="76"/>
+      <c r="D34" s="76"/>
+      <c r="E34" s="76"/>
+      <c r="F34" s="76"/>
+      <c r="G34" s="76"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="77"/>
+    </row>
+    <row r="35" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>28</v>
       </c>
@@ -18750,7 +18893,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>29</v>
       </c>
@@ -18769,7 +18912,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>30</v>
       </c>
@@ -18788,7 +18931,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>31</v>
       </c>
@@ -18807,7 +18950,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>32</v>
       </c>
@@ -18826,7 +18969,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>33</v>
       </c>
@@ -18845,7 +18988,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>34</v>
       </c>
@@ -18864,7 +19007,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>35</v>
       </c>
@@ -18883,7 +19026,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>36</v>
       </c>
@@ -18902,20 +19045,20 @@
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="73" t="s">
+    <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="75" t="s">
         <v>813</v>
       </c>
-      <c r="B44" s="74"/>
-      <c r="C44" s="74"/>
-      <c r="D44" s="74"/>
-      <c r="E44" s="74"/>
-      <c r="F44" s="74"/>
-      <c r="G44" s="74"/>
-      <c r="H44" s="74"/>
-      <c r="I44" s="75"/>
-    </row>
-    <row r="45" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="76"/>
+      <c r="C44" s="76"/>
+      <c r="D44" s="76"/>
+      <c r="E44" s="76"/>
+      <c r="F44" s="76"/>
+      <c r="G44" s="76"/>
+      <c r="H44" s="76"/>
+      <c r="I44" s="77"/>
+    </row>
+    <row r="45" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>37</v>
       </c>
@@ -18934,7 +19077,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>38</v>
       </c>
@@ -18953,7 +19096,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>39</v>
       </c>
@@ -18972,7 +19115,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>40</v>
       </c>
@@ -18991,7 +19134,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>41</v>
       </c>
@@ -19010,7 +19153,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>42</v>
       </c>
@@ -19029,7 +19172,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>43</v>
       </c>
@@ -19048,7 +19191,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>44</v>
       </c>
@@ -19067,7 +19210,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>45</v>
       </c>
@@ -19086,20 +19229,20 @@
         <v>180</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="73" t="s">
+    <row r="54" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="75" t="s">
         <v>380</v>
       </c>
-      <c r="B54" s="74"/>
-      <c r="C54" s="74"/>
-      <c r="D54" s="74"/>
-      <c r="E54" s="74"/>
-      <c r="F54" s="74"/>
-      <c r="G54" s="74"/>
-      <c r="H54" s="74"/>
-      <c r="I54" s="75"/>
-    </row>
-    <row r="55" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="76"/>
+      <c r="C54" s="76"/>
+      <c r="D54" s="76"/>
+      <c r="E54" s="76"/>
+      <c r="F54" s="76"/>
+      <c r="G54" s="76"/>
+      <c r="H54" s="76"/>
+      <c r="I54" s="77"/>
+    </row>
+    <row r="55" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>46</v>
       </c>
@@ -19118,7 +19261,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>47</v>
       </c>
@@ -19137,20 +19280,20 @@
         <v>180</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="73" t="s">
+    <row r="57" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="75" t="s">
         <v>384</v>
       </c>
-      <c r="B57" s="74"/>
-      <c r="C57" s="74"/>
-      <c r="D57" s="74"/>
-      <c r="E57" s="74"/>
-      <c r="F57" s="74"/>
-      <c r="G57" s="74"/>
-      <c r="H57" s="74"/>
-      <c r="I57" s="75"/>
-    </row>
-    <row r="58" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="76"/>
+      <c r="C57" s="76"/>
+      <c r="D57" s="76"/>
+      <c r="E57" s="76"/>
+      <c r="F57" s="76"/>
+      <c r="G57" s="76"/>
+      <c r="H57" s="76"/>
+      <c r="I57" s="77"/>
+    </row>
+    <row r="58" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>48</v>
       </c>
@@ -19169,7 +19312,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>49</v>
       </c>
@@ -19188,7 +19331,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>50</v>
       </c>
@@ -19207,7 +19350,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>51</v>
       </c>
@@ -19226,7 +19369,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>52</v>
       </c>
@@ -19245,18 +19388,18 @@
         <v>180</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="73" t="s">
+    <row r="63" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="75" t="s">
         <v>390</v>
       </c>
-      <c r="B63" s="74"/>
-      <c r="C63" s="74"/>
-      <c r="D63" s="74"/>
-      <c r="E63" s="74"/>
-      <c r="F63" s="74"/>
-      <c r="G63" s="74"/>
-      <c r="H63" s="74"/>
-      <c r="I63" s="75"/>
+      <c r="B63" s="76"/>
+      <c r="C63" s="76"/>
+      <c r="D63" s="76"/>
+      <c r="E63" s="76"/>
+      <c r="F63" s="76"/>
+      <c r="G63" s="76"/>
+      <c r="H63" s="76"/>
+      <c r="I63" s="77"/>
     </row>
     <row r="64" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
@@ -19501,17 +19644,17 @@
       </c>
     </row>
     <row r="76" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="73" t="s">
+      <c r="A76" s="75" t="s">
         <v>815</v>
       </c>
-      <c r="B76" s="74"/>
-      <c r="C76" s="74"/>
-      <c r="D76" s="74"/>
-      <c r="E76" s="74"/>
-      <c r="F76" s="74"/>
-      <c r="G76" s="74"/>
-      <c r="H76" s="74"/>
-      <c r="I76" s="75"/>
+      <c r="B76" s="76"/>
+      <c r="C76" s="76"/>
+      <c r="D76" s="76"/>
+      <c r="E76" s="76"/>
+      <c r="F76" s="76"/>
+      <c r="G76" s="76"/>
+      <c r="H76" s="76"/>
+      <c r="I76" s="77"/>
     </row>
     <row r="77" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
@@ -19685,17 +19828,17 @@
       </c>
     </row>
     <row r="86" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="73" t="s">
+      <c r="A86" s="75" t="s">
         <v>817</v>
       </c>
-      <c r="B86" s="74"/>
-      <c r="C86" s="74"/>
-      <c r="D86" s="74"/>
-      <c r="E86" s="74"/>
-      <c r="F86" s="74"/>
-      <c r="G86" s="74"/>
-      <c r="H86" s="74"/>
-      <c r="I86" s="75"/>
+      <c r="B86" s="76"/>
+      <c r="C86" s="76"/>
+      <c r="D86" s="76"/>
+      <c r="E86" s="76"/>
+      <c r="F86" s="76"/>
+      <c r="G86" s="76"/>
+      <c r="H86" s="76"/>
+      <c r="I86" s="77"/>
     </row>
     <row r="87" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
@@ -19869,17 +20012,17 @@
       </c>
     </row>
     <row r="96" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="73" t="s">
+      <c r="A96" s="75" t="s">
         <v>819</v>
       </c>
-      <c r="B96" s="74"/>
-      <c r="C96" s="74"/>
-      <c r="D96" s="74"/>
-      <c r="E96" s="74"/>
-      <c r="F96" s="74"/>
-      <c r="G96" s="74"/>
-      <c r="H96" s="74"/>
-      <c r="I96" s="75"/>
+      <c r="B96" s="76"/>
+      <c r="C96" s="76"/>
+      <c r="D96" s="76"/>
+      <c r="E96" s="76"/>
+      <c r="F96" s="76"/>
+      <c r="G96" s="76"/>
+      <c r="H96" s="76"/>
+      <c r="I96" s="77"/>
     </row>
     <row r="97" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="5">
@@ -20053,17 +20196,17 @@
       </c>
     </row>
     <row r="106" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="73" t="s">
+      <c r="A106" s="75" t="s">
         <v>821</v>
       </c>
-      <c r="B106" s="74"/>
-      <c r="C106" s="74"/>
-      <c r="D106" s="74"/>
-      <c r="E106" s="74"/>
-      <c r="F106" s="74"/>
-      <c r="G106" s="74"/>
-      <c r="H106" s="74"/>
-      <c r="I106" s="75"/>
+      <c r="B106" s="76"/>
+      <c r="C106" s="76"/>
+      <c r="D106" s="76"/>
+      <c r="E106" s="76"/>
+      <c r="F106" s="76"/>
+      <c r="G106" s="76"/>
+      <c r="H106" s="76"/>
+      <c r="I106" s="77"/>
     </row>
     <row r="107" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="5">
@@ -20237,17 +20380,17 @@
       </c>
     </row>
     <row r="116" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="73" t="s">
+      <c r="A116" s="75" t="s">
         <v>823</v>
       </c>
-      <c r="B116" s="74"/>
-      <c r="C116" s="74"/>
-      <c r="D116" s="74"/>
-      <c r="E116" s="74"/>
-      <c r="F116" s="74"/>
-      <c r="G116" s="74"/>
-      <c r="H116" s="74"/>
-      <c r="I116" s="75"/>
+      <c r="B116" s="76"/>
+      <c r="C116" s="76"/>
+      <c r="D116" s="76"/>
+      <c r="E116" s="76"/>
+      <c r="F116" s="76"/>
+      <c r="G116" s="76"/>
+      <c r="H116" s="76"/>
+      <c r="I116" s="77"/>
     </row>
     <row r="117" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="5">
@@ -20418,6 +20561,11 @@
       <c r="H125" s="24"/>
       <c r="I125" s="5" t="s">
         <v>180</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126" s="84">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -20472,29 +20620,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="72"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
+      <c r="A2" s="74"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
     </row>
     <row r="3" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
@@ -20527,17 +20675,17 @@
       <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="80" t="s">
         <v>805</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
     </row>
     <row r="5" spans="1:14" s="8" customFormat="1" ht="255" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
@@ -20731,17 +20879,17 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="78" t="s">
+      <c r="A14" s="80" t="s">
         <v>655</v>
       </c>
-      <c r="B14" s="78"/>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="78"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="80"/>
+      <c r="I14" s="80"/>
     </row>
     <row r="15" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
@@ -20933,17 +21081,17 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="79" t="s">
+      <c r="A24" s="81" t="s">
         <v>665</v>
       </c>
-      <c r="B24" s="79"/>
-      <c r="C24" s="79"/>
-      <c r="D24" s="79"/>
-      <c r="E24" s="79"/>
-      <c r="F24" s="79"/>
-      <c r="G24" s="79"/>
-      <c r="H24" s="79"/>
-      <c r="I24" s="79"/>
+      <c r="B24" s="81"/>
+      <c r="C24" s="81"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="81"/>
+      <c r="G24" s="81"/>
+      <c r="H24" s="81"/>
+      <c r="I24" s="81"/>
     </row>
     <row r="25" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
@@ -21282,17 +21430,17 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="79" t="s">
+      <c r="A41" s="81" t="s">
         <v>682</v>
       </c>
-      <c r="B41" s="79"/>
-      <c r="C41" s="79"/>
-      <c r="D41" s="79"/>
-      <c r="E41" s="79"/>
-      <c r="F41" s="79"/>
-      <c r="G41" s="79"/>
-      <c r="H41" s="79"/>
-      <c r="I41" s="79"/>
+      <c r="B41" s="81"/>
+      <c r="C41" s="81"/>
+      <c r="D41" s="81"/>
+      <c r="E41" s="81"/>
+      <c r="F41" s="81"/>
+      <c r="G41" s="81"/>
+      <c r="H41" s="81"/>
+      <c r="I41" s="81"/>
     </row>
     <row r="42" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
@@ -23932,29 +24080,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="80">
+      <c r="A1" s="73">
         <v>5</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
       <c r="L1" s="14"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="80"/>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
+      <c r="A2" s="73"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
     </row>
     <row r="3" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="48" t="s">
@@ -23987,17 +24135,17 @@
       <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="80" t="s">
         <v>805</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="78"/>
-      <c r="I4" s="78"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
     </row>
     <row r="5" spans="1:14" s="8" customFormat="1" ht="255" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
@@ -24189,17 +24337,17 @@
       </c>
     </row>
     <row r="14" spans="1:14" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="78" t="s">
+      <c r="A14" s="80" t="s">
         <v>655</v>
       </c>
-      <c r="B14" s="78"/>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="78"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="80"/>
+      <c r="I14" s="80"/>
     </row>
     <row r="15" spans="1:14" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
@@ -24391,17 +24539,17 @@
       </c>
     </row>
     <row r="24" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="79" t="s">
+      <c r="A24" s="81" t="s">
         <v>665</v>
       </c>
-      <c r="B24" s="79"/>
-      <c r="C24" s="79"/>
-      <c r="D24" s="79"/>
-      <c r="E24" s="79"/>
-      <c r="F24" s="79"/>
-      <c r="G24" s="79"/>
-      <c r="H24" s="79"/>
-      <c r="I24" s="79"/>
+      <c r="B24" s="81"/>
+      <c r="C24" s="81"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="81"/>
+      <c r="G24" s="81"/>
+      <c r="H24" s="81"/>
+      <c r="I24" s="81"/>
     </row>
     <row r="25" spans="1:9" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
@@ -24740,17 +24888,17 @@
       </c>
     </row>
     <row r="41" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="79" t="s">
+      <c r="A41" s="81" t="s">
         <v>682</v>
       </c>
-      <c r="B41" s="79"/>
-      <c r="C41" s="79"/>
-      <c r="D41" s="79"/>
-      <c r="E41" s="79"/>
-      <c r="F41" s="79"/>
-      <c r="G41" s="79"/>
-      <c r="H41" s="79"/>
-      <c r="I41" s="79"/>
+      <c r="B41" s="81"/>
+      <c r="C41" s="81"/>
+      <c r="D41" s="81"/>
+      <c r="E41" s="81"/>
+      <c r="F41" s="81"/>
+      <c r="G41" s="81"/>
+      <c r="H41" s="81"/>
+      <c r="I41" s="81"/>
     </row>
     <row r="42" spans="1:9" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
@@ -27303,11 +27451,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C4:C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27324,28 +27472,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="77"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
     </row>
     <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="52" t="s">
@@ -27376,33 +27524,25 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>1</v>
-      </c>
-      <c r="B4" s="54" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="54" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="54" t="s">
-        <v>628</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>627</v>
-      </c>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="85" t="s">
+        <v>985</v>
+      </c>
+      <c r="B4" s="86"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="87"/>
     </row>
     <row r="5" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="54" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" s="54" t="s">
         <v>33</v>
@@ -27418,15 +27558,15 @@
         <v>627</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="54" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D6" s="55"/>
       <c r="E6" s="55"/>
@@ -27439,12 +27579,12 @@
         <v>627</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="54" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="54" t="s">
         <v>37</v>
@@ -27460,12 +27600,12 @@
         <v>627</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="54" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C8" s="54" t="s">
         <v>37</v>
@@ -27481,15 +27621,15 @@
         <v>627</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="54" t="s">
-        <v>626</v>
+        <v>37</v>
       </c>
       <c r="D9" s="55"/>
       <c r="E9" s="55"/>
@@ -27502,15 +27642,15 @@
         <v>627</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="54" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="D10" s="55"/>
       <c r="E10" s="55"/>
@@ -27525,13 +27665,13 @@
     </row>
     <row r="11" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="54" t="s">
-        <v>42</v>
+        <v>625</v>
       </c>
       <c r="D11" s="55"/>
       <c r="E11" s="55"/>
@@ -27544,44 +27684,237 @@
         <v>627</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
+    <row r="12" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>8</v>
+      </c>
+      <c r="B12" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="55"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="54" t="s">
+        <v>628</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>627</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
+      <c r="A13" s="88" t="s">
+        <v>986</v>
+      </c>
+      <c r="B13" s="88"/>
+      <c r="C13" s="88"/>
+      <c r="D13" s="88"/>
+      <c r="E13" s="88"/>
+      <c r="F13" s="88"/>
+      <c r="G13" s="88"/>
+      <c r="H13" s="88"/>
+      <c r="I13" s="88"/>
+    </row>
+    <row r="14" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>9</v>
+      </c>
+      <c r="B14" s="54" t="s">
+        <v>987</v>
+      </c>
+      <c r="C14" s="89" t="s">
+        <v>994</v>
+      </c>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="54" t="s">
+        <v>628</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>10</v>
+      </c>
+      <c r="B15" s="54" t="s">
+        <v>988</v>
+      </c>
+      <c r="C15" s="89" t="s">
+        <v>994</v>
+      </c>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="54" t="s">
+        <v>628</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>11</v>
+      </c>
+      <c r="B16" s="54" t="s">
+        <v>989</v>
+      </c>
+      <c r="C16" s="54" t="s">
+        <v>995</v>
+      </c>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="54" t="s">
+        <v>628</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>12</v>
+      </c>
+      <c r="B17" s="54" t="s">
+        <v>990</v>
+      </c>
+      <c r="C17" s="54" t="s">
+        <v>995</v>
+      </c>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="54" t="s">
+        <v>628</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>13</v>
+      </c>
+      <c r="B18" s="54" t="s">
+        <v>996</v>
+      </c>
+      <c r="C18" s="54" t="s">
+        <v>995</v>
+      </c>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="54" t="s">
+        <v>628</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>14</v>
+      </c>
+      <c r="B19" s="54" t="s">
+        <v>991</v>
+      </c>
+      <c r="C19" s="54" t="s">
+        <v>998</v>
+      </c>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="54" t="s">
+        <v>628</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="32">
+        <v>15</v>
+      </c>
+      <c r="B20" s="54" t="s">
+        <v>992</v>
+      </c>
+      <c r="C20" s="54" t="s">
+        <v>997</v>
+      </c>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="54" t="s">
+        <v>628</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="32">
+        <v>16</v>
+      </c>
+      <c r="B21" s="54" t="s">
+        <v>993</v>
+      </c>
+      <c r="C21" s="54" t="s">
+        <v>999</v>
+      </c>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="54" t="s">
+        <v>628</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="32">
+        <v>17</v>
+      </c>
+      <c r="B22" s="54" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C22" s="54" t="s">
+        <v>997</v>
+      </c>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="54" t="s">
+        <v>628</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>627</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:I2"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A13:I13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -27607,28 +27940,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="77"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="77"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
     </row>
     <row r="3" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="52" t="s">

</xml_diff>